<commit_message>
Updated text & better layout in the cover sheet. Removed mention of tabs not present in the FDA version.
</commit_message>
<xml_diff>
--- a/templates/excel/fda-template.xlsx
+++ b/templates/excel/fda-template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F86A5A6-98DE-2846-904D-83DCFDA73CB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E300068D-57B5-1447-BD8B-88F6CFF253B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" activeTab="7" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
+    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cover" sheetId="4" r:id="rId1"/>
+    <sheet name="Cover" sheetId="16" r:id="rId1"/>
     <sheet name="Glossary" sheetId="1" r:id="rId2"/>
     <sheet name="Software Requirements" sheetId="6" r:id="rId3"/>
     <sheet name="Traceability Report" sheetId="14" r:id="rId4"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="256">
   <si>
     <t>Term</t>
   </si>
@@ -577,22 +577,6 @@
   </si>
   <si>
     <t>Tidepool Loop 1.0.0 Requirements, Traceability, Hazard Analysis and Verification Reports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-This document is intended to show the detail of the Tidepool’s Quality Management System for Tidepool Loop. The document was automatically generated from Tidepool’s quality management system. The source documents are in Jira, our project management system. Information was pulled from these projects:
-• Tidepool Loop Functional Requirements - TLFR
-• Tidepool Loop Risks - TLR
-• Tidepool Loop Work Tickets - LOOP
-Tabs in this spreadsheet:
-• Software Requirements: This spreadsheet tab contains all software requirements for Tidepool Loop, as derived from the Tidepool Loop Functional Requirements (TLFR) Jira project.
-• Traceability Summary: This spreadsheet tab summarizes traceability from requirements to implementation and verification summary. It does not include risk analysis for each requirement.
-• Traceability Report: This spreadsheet tab demonstrates traceability to and from all Tidepool Loop functional requirements. It has columns for each requirement, associated risks, design and development, verification tests, and test status.
-  • For more information on Tidepool Loop’s requirements, please see Section 16 of the main pre-marketing notification document.
-• Full Traceability Report: This spreadsheet tab includes all of the above information, but also includes traceability to all risk management issues.
-• Hazard Analysis: This spreadsheet tab demonstrates Tidepool’s Risk and Hazard analysis of Tidepool Loop. Columns are included for each risk, including a summary, the potential harm and hazard category, risk assessment prior to mitigation, details of any mitigation, and risk assessment post-mitigation.
-• Unresolved Defects: This spreadsheet lists all unresolved defects and anomalies (open bugs) for Tidepool Loop 1.0.0.
-• Automated Tests: This spreadsheet lists additional verification testing performed via test automation methods.</t>
   </si>
   <si>
     <t>Automatically generated on {timestamp}</t>
@@ -842,6 +826,66 @@
   </si>
   <si>
     <t>&lt;&lt;&lt;insert: bugs_list('empty': 'No unresolved defects')&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• </t>
+  </si>
+  <si>
+    <t>Risk Matrix</t>
+  </si>
+  <si>
+    <t>Risk Scoring</t>
+  </si>
+  <si>
+    <t>Glossary</t>
+  </si>
+  <si>
+    <t>Cover</t>
+  </si>
+  <si>
+    <t>The tabs in this workbook are:</t>
+  </si>
+  <si>
+    <t>Tidepool Loop Instructions for Use - IFU</t>
+  </si>
+  <si>
+    <t>Tidepool Loop Work Tickets - LOOP</t>
+  </si>
+  <si>
+    <t>Tidepool Loop Risks - TLR</t>
+  </si>
+  <si>
+    <t>Tidepool Loop Functional Requirements - TLFR</t>
+  </si>
+  <si>
+    <t>This document is intended to show the detail of the Tidepool’s Quality Management System for Tidepool Loop. The document was automatically generated from Tidepool’s quality management system. The source documents are in Jira, our project management system. Information was pulled from these projects:</t>
+  </si>
+  <si>
+    <t>This tab.</t>
+  </si>
+  <si>
+    <t>Glossary of terms used in the other tab.</t>
+  </si>
+  <si>
+    <t>This tab contains all software requirements for Tidepool Loop, as derived from the Tidepool Loop Functional Requirements (TLFR) Jira project.</t>
+  </si>
+  <si>
+    <t>This tab demonstrates traceability to and from all Tidepool Loop functional requirements. It has columns for each requirement, associated risks, design and development, verification tests, and test status. For more information on Tidepool Loop’s requirements, please see Section 16 of the main pre-marketing notification document.</t>
+  </si>
+  <si>
+    <t>This tab shows Tidepool's risk severity and probability scoring criteria.</t>
+  </si>
+  <si>
+    <t>This tab shows Tidepool's risk assessment matrix.</t>
+  </si>
+  <si>
+    <t>This tab demonstrates Tidepool’s Risk and Hazard analysis of Tidepool Loop. Columns are included for each risk, including a summary, the potential harm and hazard category, risk assessment prior to mitigation, details of any mitigation, and risk assessment post-mitigation.</t>
+  </si>
+  <si>
+    <t>This tab lists all unresolved defects and anomalies (open bugs) for Tidepool Loop 1.0.0.</t>
+  </si>
+  <si>
+    <t>This tab lists additional verification testing performed via test automation methods.</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1112,12 +1156,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1215,6 +1253,31 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1529,42 +1592,205 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3189D35B-773B-1A43-B76D-B05EF339D4EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694C0506-66E0-A540-8343-72013670FB41}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="120.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="93.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="52" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="53" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="49"/>
+    </row>
+    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="49"/>
+    </row>
+    <row r="3" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="265" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>177</v>
+      <c r="B3" s="54"/>
+      <c r="C3" s="49"/>
+    </row>
+    <row r="4" spans="1:3" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="C5" s="50"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" s="50"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="C7" s="50"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="C8" s="50"/>
+    </row>
+    <row r="9" spans="1:3" s="47" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+    </row>
+    <row r="10" spans="1:3" s="47" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="47" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="42" x14ac:dyDescent="0.2">
+      <c r="A16" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="46" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="99" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1595,535 +1821,535 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="A1" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="35"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="35"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="33"/>
+      <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="35"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="35"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="33"/>
+      <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>226</v>
+      <c r="C12" s="18" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="33"/>
+      <c r="B13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="33"/>
+      <c r="B14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="33"/>
+      <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="33"/>
+      <c r="B17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="18" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="33"/>
+      <c r="B18" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="18" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="18"/>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="35"/>
-      <c r="B22" s="19" t="s">
+      <c r="A22" s="33"/>
+      <c r="B22" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="35"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="33"/>
+      <c r="B25" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="18" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="35"/>
-      <c r="B26" s="19" t="s">
+      <c r="A26" s="33"/>
+      <c r="B26" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="18" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="35"/>
-      <c r="B27" s="19" t="s">
+      <c r="A27" s="33"/>
+      <c r="B27" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
-      <c r="B28" s="19" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="18" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
-      <c r="B29" s="19" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="35"/>
-      <c r="B30" s="19" t="s">
+      <c r="A30" s="33"/>
+      <c r="B30" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="20"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="18"/>
     </row>
     <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="20"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="18"/>
     </row>
     <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="35"/>
-      <c r="B34" s="19" t="s">
+      <c r="A34" s="33"/>
+      <c r="B34" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="18" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="35"/>
-      <c r="B36" s="19" t="s">
+      <c r="A36" s="33"/>
+      <c r="B36" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="18" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="18" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="20"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="18"/>
     </row>
     <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="18" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="35"/>
-      <c r="B40" s="19" t="s">
+      <c r="A40" s="33"/>
+      <c r="B40" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="18" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A41" s="35"/>
-      <c r="B41" s="19" t="s">
+      <c r="A41" s="33"/>
+      <c r="B41" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="18" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A42" s="35"/>
-      <c r="B42" s="19" t="s">
+      <c r="A42" s="33"/>
+      <c r="B42" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="33"/>
+      <c r="B43" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="18"/>
+    </row>
+    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A44" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="16"/>
+      <c r="C44" s="18"/>
+    </row>
+    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A45" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="18"/>
+    </row>
+    <row r="46" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A46" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="20" x14ac:dyDescent="0.2">
+      <c r="A47" s="20"/>
+      <c r="B47" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="20"/>
+      <c r="B48" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A49" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="20"/>
+      <c r="B50" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" s="20"/>
+      <c r="B51" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="20"/>
+      <c r="B52" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="20"/>
+      <c r="B53" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A55" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="16"/>
+      <c r="C55" s="18"/>
+    </row>
+    <row r="56" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A56" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="18" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="35"/>
-      <c r="B43" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="20"/>
-    </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A44" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="20"/>
-    </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="20"/>
-    </row>
-    <row r="46" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A46" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A47" s="22"/>
-      <c r="B47" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="22"/>
-      <c r="B48" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="22"/>
-      <c r="B50" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="22"/>
-      <c r="B51" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="22"/>
-      <c r="B52" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="22"/>
-      <c r="B53" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A55" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="20"/>
-    </row>
-    <row r="56" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A56" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>181</v>
-      </c>
-    </row>
     <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="20"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="18"/>
     </row>
     <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A58" s="21" t="s">
+      <c r="A58" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="20"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="18"/>
     </row>
     <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="20"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2169,30 +2395,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="A1" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2231,8 +2457,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>228</v>
+      <c r="A1" s="21" t="s">
+        <v>227</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2244,37 +2470,37 @@
       <c r="I1" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="9" t="s">
         <v>197</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2309,256 +2535,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="29">
+      <c r="A4" s="27">
         <v>5</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="39">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="36" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="18" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
-      <c r="B6" s="20" t="s">
+      <c r="A6" s="38"/>
+      <c r="B6" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="20" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="18" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="18" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="39">
+      <c r="A8" s="37">
         <v>3</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="36" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="38"/>
+      <c r="B9" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="20" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="18" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="18" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="39">
+      <c r="A11" s="37">
         <v>2</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="36" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="18" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="38"/>
+      <c r="B12" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="35"/>
+      <c r="D12" s="18" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="41"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="20" t="s">
+      <c r="C13" s="36"/>
+      <c r="D13" s="18" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="39">
+      <c r="A14" s="37">
         <v>1</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="36" t="s">
+      <c r="B14" s="18"/>
+      <c r="C14" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="18" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="20" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="18" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="41"/>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="20" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="18" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
     </row>
     <row r="20" spans="1:4" ht="126" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="26" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A21" s="30">
+      <c r="A21" s="28">
         <v>5</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="30">
+      <c r="A22" s="28">
         <v>4</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" s="30">
+      <c r="A23" s="28">
         <v>3</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="18" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A24" s="30">
+      <c r="A24" s="28">
         <v>2</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="18" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="30">
+      <c r="A25" s="28">
         <v>1</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="18" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2600,15 +2826,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -2619,36 +2845,36 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="30" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>168</v>
       </c>
       <c r="C5" s="3"/>
@@ -2658,8 +2884,8 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="43"/>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="41"/>
+      <c r="B6" s="29" t="s">
         <v>169</v>
       </c>
       <c r="C6" s="5"/>
@@ -2669,8 +2895,8 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="43"/>
-      <c r="B7" s="31" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="29" t="s">
         <v>170</v>
       </c>
       <c r="C7" s="5"/>
@@ -2680,8 +2906,8 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="43"/>
-      <c r="B8" s="31" t="s">
+      <c r="A8" s="41"/>
+      <c r="B8" s="29" t="s">
         <v>171</v>
       </c>
       <c r="C8" s="5"/>
@@ -2691,8 +2917,8 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
-      <c r="B9" s="31" t="s">
+      <c r="A9" s="42"/>
+      <c r="B9" s="29" t="s">
         <v>172</v>
       </c>
       <c r="C9" s="5"/>
@@ -2744,104 +2970,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="J1" s="13" t="s">
+      <c r="A1" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="P1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J2" s="12" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J2" s="14" t="s">
+      <c r="P2" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="P2" s="14" t="s">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J3" s="13" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J3" s="15" t="s">
+      <c r="P3" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="P3" s="15" t="s">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J4" s="10" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J4" s="12" t="s">
+      <c r="P4" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="P4" s="12" t="s">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J5" s="14" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J5" s="16" t="s">
+      <c r="P5" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="P5" s="16" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="J7" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="M7" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="N7" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="O7" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="P7" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="Q7" s="9" t="s">
         <v>224</v>
-      </c>
-      <c r="Q7" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2862,7 +3088,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2875,30 +3101,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="A1" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>190</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2933,34 +3159,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="A1" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>188</v>
+      <c r="E3" s="9" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change "Unresolved Defects" to "Unresolved Anomalies"
</commit_message>
<xml_diff>
--- a/templates/excel/fda-template.xlsx
+++ b/templates/excel/fda-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E300068D-57B5-1447-BD8B-88F6CFF253B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB47A3E-A543-984D-AE85-EF27D4F6E772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
+    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" activeTab="7" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="16" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="Risk Scoring" sheetId="2" r:id="rId5"/>
     <sheet name="Risk Matrix" sheetId="3" r:id="rId6"/>
     <sheet name="Hazard Analysis" sheetId="10" r:id="rId7"/>
-    <sheet name="Unresolved Defects" sheetId="12" r:id="rId8"/>
+    <sheet name="Unresolved Anomalies" sheetId="12" r:id="rId8"/>
     <sheet name="Automated Tests" sheetId="13" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Automated Tests'!$A$3:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Unresolved Defects'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Unresolved Anomalies'!$A$3:$D$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="257">
   <si>
     <t>Term</t>
   </si>
@@ -825,9 +825,6 @@
     <t>&lt;&lt;&lt;insert: tests_list()&gt;&gt;&gt;</t>
   </si>
   <si>
-    <t>&lt;&lt;&lt;insert: bugs_list('empty': 'No unresolved defects')&gt;&gt;&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">• </t>
   </si>
   <si>
@@ -886,6 +883,12 @@
   </si>
   <si>
     <t>This tab lists additional verification testing performed via test automation methods.</t>
+  </si>
+  <si>
+    <t>Unresolved Anomalies</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;insert: bugs_list('empty': 'No unresolved anomalies')&gt;&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -1211,6 +1214,31 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1253,31 +1281,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1598,7 +1601,7 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1610,173 +1613,173 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
     </row>
     <row r="4" spans="1:3" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="33"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" s="33"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="C7" s="33"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="33"/>
+    </row>
+    <row r="9" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+    </row>
+    <row r="10" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>245</v>
-      </c>
-      <c r="C5" s="50"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="C6" s="50"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>243</v>
-      </c>
-      <c r="C7" s="50"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>242</v>
-      </c>
-      <c r="C8" s="50"/>
-    </row>
-    <row r="9" spans="1:3" s="47" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48" t="s">
-        <v>241</v>
-      </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-    </row>
-    <row r="10" spans="1:3" s="47" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="C10" s="8" t="s">
+    </row>
+    <row r="11" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="47" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>248</v>
-      </c>
-    </row>
     <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
-        <v>236</v>
+      <c r="A12" s="31" t="s">
+        <v>235</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>226</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
-        <v>236</v>
+      <c r="A13" s="31" t="s">
+        <v>235</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>227</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="46" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>252</v>
-      </c>
-    </row>
     <row r="16" spans="1:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
-        <v>236</v>
+      <c r="A16" s="31" t="s">
+        <v>235</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>228</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
-        <v>236</v>
+      <c r="A17" s="31" t="s">
+        <v>235</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>229</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
-        <v>236</v>
+      <c r="A18" s="31" t="s">
+        <v>235</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>230</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -1821,11 +1824,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="40" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -1842,7 +1845,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="41" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -1853,7 +1856,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="33"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
@@ -1862,7 +1865,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="33"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
@@ -1871,7 +1874,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="41" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="17" t="s">
@@ -1882,7 +1885,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="17" t="s">
         <v>12</v>
       </c>
@@ -1891,7 +1894,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="41" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="17" t="s">
@@ -1902,7 +1905,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="33"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="17" t="s">
         <v>17</v>
       </c>
@@ -1911,7 +1914,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="17" t="s">
         <v>19</v>
       </c>
@@ -1920,7 +1923,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.2">
-      <c r="A12" s="33"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
@@ -1929,7 +1932,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="33"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="17" t="s">
         <v>22</v>
       </c>
@@ -1938,7 +1941,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="33"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="17" t="s">
         <v>24</v>
       </c>
@@ -1947,7 +1950,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="33"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
@@ -1956,7 +1959,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="41" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="17" t="s">
@@ -1967,7 +1970,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="33"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="17" t="s">
         <v>31</v>
       </c>
@@ -1976,7 +1979,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="17" t="s">
         <v>33</v>
       </c>
@@ -2003,7 +2006,7 @@
       <c r="C20" s="18"/>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="41" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="17" t="s">
@@ -2014,7 +2017,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="33"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="17" t="s">
         <v>42</v>
       </c>
@@ -2030,7 +2033,7 @@
       <c r="C23" s="18"/>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="41" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -2041,7 +2044,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="33"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="17" t="s">
         <v>48</v>
       </c>
@@ -2050,7 +2053,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="33"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="17" t="s">
         <v>50</v>
       </c>
@@ -2059,7 +2062,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="17" t="s">
         <v>52</v>
       </c>
@@ -2068,7 +2071,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="33"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="17" t="s">
         <v>54</v>
       </c>
@@ -2077,7 +2080,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="33"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="17" t="s">
         <v>56</v>
       </c>
@@ -2086,7 +2089,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="17" t="s">
         <v>58</v>
       </c>
@@ -2109,7 +2112,7 @@
       <c r="C32" s="18"/>
     </row>
     <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="41" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="17" t="s">
@@ -2120,7 +2123,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="33"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="17" t="s">
         <v>65</v>
       </c>
@@ -2129,7 +2132,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="41" t="s">
         <v>67</v>
       </c>
       <c r="B35" s="17" t="s">
@@ -2140,7 +2143,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="33"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="17" t="s">
         <v>70</v>
       </c>
@@ -2167,7 +2170,7 @@
       <c r="C38" s="18"/>
     </row>
     <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="41" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="17" t="s">
@@ -2178,7 +2181,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="33"/>
+      <c r="A40" s="42"/>
       <c r="B40" s="17" t="s">
         <v>79</v>
       </c>
@@ -2187,7 +2190,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A41" s="33"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="17" t="s">
         <v>81</v>
       </c>
@@ -2196,7 +2199,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A42" s="33"/>
+      <c r="A42" s="42"/>
       <c r="B42" s="17" t="s">
         <v>83</v>
       </c>
@@ -2205,7 +2208,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="33"/>
+      <c r="A43" s="42"/>
       <c r="B43" s="17" t="s">
         <v>84</v>
       </c>
@@ -2569,11 +2572,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="37">
+      <c r="A5" s="46">
         <v>4</v>
       </c>
       <c r="B5" s="18"/>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="43" t="s">
         <v>119</v>
       </c>
       <c r="D5" s="18" t="s">
@@ -2581,31 +2584,31 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="18" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="18" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="37">
+      <c r="A8" s="46">
         <v>3</v>
       </c>
       <c r="B8" s="18"/>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="43" t="s">
         <v>125</v>
       </c>
       <c r="D8" s="18" t="s">
@@ -2613,31 +2616,31 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="18" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="39"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="18" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="37">
+      <c r="A11" s="46">
         <v>2</v>
       </c>
       <c r="B11" s="18"/>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="43" t="s">
         <v>131</v>
       </c>
       <c r="D11" s="18" t="s">
@@ -2645,31 +2648,31 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="35"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="18" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="18" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="37">
+      <c r="A14" s="46">
         <v>1</v>
       </c>
       <c r="B14" s="18"/>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="43" t="s">
         <v>137</v>
       </c>
       <c r="D14" s="18" t="s">
@@ -2677,21 +2680,21 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="18" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
+      <c r="A16" s="48"/>
       <c r="B16" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="18" t="s">
         <v>142</v>
       </c>
@@ -2845,13 +2848,13 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="45"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="54"/>
     </row>
     <row r="4" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="30" t="s">
@@ -2871,7 +2874,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="49" t="s">
         <v>166</v>
       </c>
       <c r="B5" s="29" t="s">
@@ -2884,7 +2887,7 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="29" t="s">
         <v>169</v>
       </c>
@@ -2895,7 +2898,7 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="29" t="s">
         <v>170</v>
       </c>
@@ -2906,7 +2909,7 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="29" t="s">
         <v>171</v>
       </c>
@@ -2917,7 +2920,7 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="29" t="s">
         <v>172</v>
       </c>
@@ -3088,8 +3091,8 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3102,7 +3105,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -3124,7 +3127,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed column headings: "Defect" -> "Anomaly"
</commit_message>
<xml_diff>
--- a/templates/excel/fda-template.xlsx
+++ b/templates/excel/fda-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB47A3E-A543-984D-AE85-EF27D4F6E772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C6E30-FC1F-9141-A689-A1FB73B74664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" activeTab="7" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
@@ -612,12 +612,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Defect Key</t>
-  </si>
-  <si>
-    <t>Defect Summary</t>
   </si>
   <si>
     <t>Fix Version</t>
@@ -889,6 +883,12 @@
   </si>
   <si>
     <t>&lt;&lt;&lt;insert: bugs_list('empty': 'No unresolved anomalies')&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Anomaly Key</t>
+  </si>
+  <si>
+    <t>Anomaly Summary</t>
   </si>
 </sst>
 </file>
@@ -1635,151 +1635,151 @@
     </row>
     <row r="4" spans="1:3" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C5" s="33"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C6" s="33"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C7" s="33"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C8" s="33"/>
     </row>
     <row r="9" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
     </row>
     <row r="10" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>237</v>
-      </c>
       <c r="C14" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="42" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1825,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -1928,7 +1928,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2399,7 +2399,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2461,7 +2461,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2492,18 +2492,18 @@
         <v>186</v>
       </c>
       <c r="G3" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2974,103 +2974,103 @@
   <sheetData>
     <row r="1" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J2" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J3" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J4" s="10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J5" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="I7" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="L7" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="N7" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="O7" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="Q7" s="9" t="s">
         <v>222</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3092,7 +3092,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3105,7 +3105,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -3113,21 +3113,21 @@
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>188</v>
+        <v>255</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>189</v>
+        <v>256</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>187</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -3163,7 +3163,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -3172,16 +3172,16 @@
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>192</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>194</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>187</v>
@@ -3189,7 +3189,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new column "Reason for Deferral" to the "Unresolved Anomalies" tab
</commit_message>
<xml_diff>
--- a/templates/excel/fda-template.xlsx
+++ b/templates/excel/fda-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C6E30-FC1F-9141-A689-A1FB73B74664}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3235AEB7-6ED7-894A-B7FD-665CE9504F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" activeTab="7" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Automated Tests'!$A$3:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Unresolved Anomalies'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Unresolved Anomalies'!$A$3:$E$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="258">
   <si>
     <t>Term</t>
   </si>
@@ -889,6 +889,9 @@
   </si>
   <si>
     <t>Anomaly Summary</t>
+  </si>
+  <si>
+    <t>Reason for Deferral</t>
   </si>
 </sst>
 </file>
@@ -3089,7 +3092,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -3101,9 +3104,10 @@
     <col min="2" max="2" width="70.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>253</v>
       </c>
@@ -3111,7 +3115,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>255</v>
       </c>
@@ -3124,14 +3128,17 @@
       <c r="D3" s="9" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>254</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:D3" xr:uid="{8E9A8066-C04A-CE49-A6EA-5A65887ABDCE}"/>
+  <autoFilter ref="A3:E3" xr:uid="{AF851B01-A62E-CF4F-B7DC-5677CB269975}"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated glossary from Dan
</commit_message>
<xml_diff>
--- a/templates/excel/fda-template.xlsx
+++ b/templates/excel/fda-template.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC927443-E6C9-3346-8EA6-4894BB60608E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044CD715-23CE-5F45-B5D1-D0A03A5CE218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
+    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" activeTab="1" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="16" r:id="rId1"/>
-    <sheet name="Glossary" sheetId="1" r:id="rId2"/>
+    <sheet name="Glossary" sheetId="17" r:id="rId2"/>
     <sheet name="Software Requirements" sheetId="6" r:id="rId3"/>
     <sheet name="Traceability Report" sheetId="14" r:id="rId4"/>
     <sheet name="Risk Scoring" sheetId="2" r:id="rId5"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="256">
   <si>
     <t>Term</t>
   </si>
@@ -55,12 +55,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>ACE_PUMP / pump</t>
-  </si>
-  <si>
-    <t>“Alternate Controller Enabled” insulin pump.</t>
-  </si>
-  <si>
     <t>ACTIVE_CARBS</t>
   </si>
   <si>
@@ -76,33 +70,12 @@
     <t>B</t>
   </si>
   <si>
-    <t>BOLUS/bolus</t>
-  </si>
-  <si>
-    <t>A one-time dose of insulin given to bring down high glucose or cover an expected rise in glucose from eating.</t>
-  </si>
-  <si>
-    <t>BG/Glucose</t>
-  </si>
-  <si>
-    <t>Glucose measurement.</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>CALIBRATION_GLUCOSE_VALUE </t>
-  </si>
-  <si>
-    <t>Glucose value measured thru a blood sample to optimize system performance.</t>
-  </si>
-  <si>
     <t>CARBOHYDRATE_TO_INSULIN_RATIO</t>
   </si>
   <si>
-    <t>The amount of insulin needed to cover a given amount of carbohydrates. Expressed in (gU).</t>
-  </si>
-  <si>
     <t>CORRECTION_RANGE</t>
   </si>
   <si>
@@ -136,15 +109,6 @@
     <t>DELIVERY_LIMITS </t>
   </si>
   <si>
-    <t>Safety guardrails for your insulin delivery.</t>
-  </si>
-  <si>
-    <t>DOSING_SAFETY_THRESHOLD </t>
-  </si>
-  <si>
-    <t>Equivalent to the user's SUSPEND_THRESHOLD setting for the first half of the INSULIN_ACTIVITY_DURATION, and then linearly increases until it reaches the midpoint of the CORRECTION_RANGE at the end of the INSULIN_ACTIVITY_DURATION.</t>
-  </si>
-  <si>
     <t>DOSING_UNCERTAINTY </t>
   </si>
   <si>
@@ -205,9 +169,6 @@
     <t>INSULIN_ACTIVITY_DURATION </t>
   </si>
   <si>
-    <t>The amount of time insulin is active in the body. Tidepool Loop sets this time to 6 hours.</t>
-  </si>
-  <si>
     <t>INSULIN_ACTION_PEAK </t>
   </si>
   <si>
@@ -250,9 +211,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>MAXIUMUM_BASAL_RATE </t>
-  </si>
-  <si>
     <t>The maximum amount of basal insulin that the pump can be programmed to deliver by either the user or Tidepool Loop’s algorithm to deliver per hour. </t>
   </si>
   <si>
@@ -280,9 +238,6 @@
     <t>PREDICTED_GLUCOSE </t>
   </si>
   <si>
-    <t>Forecast of future glucose values that spans from the current time to to td, some time in the future.</t>
-  </si>
-  <si>
     <t>PREDICTIVE_ALERTS</t>
   </si>
   <si>
@@ -322,9 +277,6 @@
     <t>Icon that allows you to see if automation is on and working.</t>
   </si>
   <si>
-    <t xml:space="preserve">SUSPEND_THRESHOLD / GLUCOSE_SAFETY_THRESHOLD </t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -364,9 +316,6 @@
     <t>USER_NOTIFICATION/notification</t>
   </si>
   <si>
-    <t>User-facing notifications communicating important information to Tidepool Loop Users. Notifications can be delivered as Alerts or Alarms.</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -583,14 +532,6 @@
     <t>Corresponds with Tidepool Loop 1.0.0 (build {build_number})</t>
   </si>
   <si>
-    <t>Feature telling Tidepool Loop to adjust your basal insulin and lower your glucose CORRECTION_RANGE in advance of your meal.
-The temp adjust will be in effect for up to one hour or until you cancel it or enter your next Carb Entry.</t>
-  </si>
-  <si>
-    <t>Feature telling Tidepool Loop to adjust both your basal insulin and your glucose CORRECTION_RANGE to help you meet your glucose goals during that activity.
-Workout temp adjust will be in effect for the time you indicate when you activate it or until you cancel it.</t>
-  </si>
-  <si>
     <t>Req ID</t>
   </si>
   <si>
@@ -705,79 +646,6 @@
     <t>Benefit outweigh Risks? Y/N</t>
   </si>
   <si>
-    <r>
-      <t>From t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> to t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>d/2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>, the correction target is equal to the SUSPEND_THRESHOLD. From t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>d/2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> to t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>, the correction target is a linear blend over time of the SUSPEND_THRESHOLD and the average of the correction maximum and correction minimum.</t>
-    </r>
-  </si>
-  <si>
     <t>Software Requirements</t>
   </si>
   <si>
@@ -869,13 +737,88 @@
   </si>
   <si>
     <t>Reason for Deferral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACE_PUMP </t>
+  </si>
+  <si>
+    <t>“Alternate Controller Enabled” insulin pump. Any documentation with “pump” or “insulin pump” are references to ACE_PUMP.</t>
+  </si>
+  <si>
+    <t>BOLUS</t>
+  </si>
+  <si>
+    <t>A one-time dose of insulin given to bring down high glucose or cover an expected rise in glucose from eating. Any documentation with “bolus” is reference to BOLUS.</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>Blood glucose values measured only by Self-monitoring of blood glucose(eg Blood Glucose Meter).</t>
+  </si>
+  <si>
+    <t>CALIBRATION_GLUCOSE </t>
+  </si>
+  <si>
+    <t>Glucose value measured thru a sample to optimize system performance.</t>
+  </si>
+  <si>
+    <t>The amount of insulin needed to cover a given amount of carbohydrates. Expressed in (g/U).</t>
+  </si>
+  <si>
+    <t>The minimum value and upper or maximum value of CORRECTION_RANGE that are averaged together.</t>
+  </si>
+  <si>
+    <t>Safety guardrails for insulin delivery.</t>
+  </si>
+  <si>
+    <t>DOSING_SAFETY_THRESHOLD</t>
+  </si>
+  <si>
+    <t>Equivalent to the user's GLUCOSE_SAFETY_LIMIT setting for the first half of the INSULIN_ACTIVITY_DURATION, and then linearly increases until it reaches the midpoint of the CORRECTION_RANGE at the end of the INSULIN_ACTIVITY_DURATION.</t>
+  </si>
+  <si>
+    <t>ESTIMATED_GLUCOSE_VALUE</t>
+  </si>
+  <si>
+    <t>CGM glucose measurement</t>
+  </si>
+  <si>
+    <t>The amount of time insulin is active in the body.</t>
+  </si>
+  <si>
+    <t>MAXIMUM_BASAL_RATE </t>
+  </si>
+  <si>
+    <t>Forecast of future glucose values that spans from the current time to some time in the future.</t>
+  </si>
+  <si>
+    <t>Feature telling Tidepool Loop to adjust your basal insulin and lower your glucose CORRECTION_RANGE in advance of your meal. The temp adjust will be in effect for up to one hour or until you cancel it or enter your next Carb Entry.</t>
+  </si>
+  <si>
+    <t>SAFETY_DOSING_THRESHOLD</t>
+  </si>
+  <si>
+    <t>SENSOR_GLUCOSE</t>
+  </si>
+  <si>
+    <t>CGM glucose measurements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUSPEND_THRESHOLD / GLUCOSE_SAFETY_LIMIT </t>
+  </si>
+  <si>
+    <t>User-facing notifications communicating important information to Tidepool Loop Users. Notifications can be delivered as Alerts or Alarms. Any documentation with “notification” is reference to USER_NOTIFICATION.</t>
+  </si>
+  <si>
+    <t>Feature telling Tidepool Loop to adjust both your basal insulin and your glucose CORRECTION_RANGE to help you meet your glucose goals during that activity. Workout temp adjust will be in effect for the time you indicate when you activate it or until you cancel it.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -965,12 +908,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <vertAlign val="subscript"/>
-      <sz val="12"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color rgb="FFFFFFFF"/>
@@ -989,6 +926,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1124,7 +1074,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1160,18 +1110,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1179,19 +1120,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1219,48 +1160,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1581,7 +1543,7 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
@@ -1593,162 +1555,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
-        <v>176</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="37"/>
+      <c r="A1" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
+      <c r="A2" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:3" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="C5" s="33"/>
+      <c r="A5" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" s="28"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="C6" s="33"/>
+      <c r="A6" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="28"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="C7" s="33"/>
+      <c r="A7" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="C7" s="28"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" s="33"/>
-    </row>
-    <row r="9" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-    </row>
-    <row r="10" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
-        <v>227</v>
+      <c r="A8" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" s="28"/>
+    </row>
+    <row r="9" spans="1:3" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+    </row>
+    <row r="10" spans="1:3" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="32" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
-        <v>227</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
-        <v>227</v>
+      <c r="A12" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
-        <v>227</v>
+      <c r="A13" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>241</v>
-      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
-        <v>227</v>
+      <c r="A14" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
-        <v>227</v>
+      <c r="A15" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
-        <v>227</v>
+      <c r="A16" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
-        <v>227</v>
+      <c r="A17" s="26" t="s">
+        <v>207</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -1774,14 +1736,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C10F0E1-442D-A543-BEAE-432F30748801}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716CC299-C6E7-6146-937F-CC97AAC67C2B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1793,16 +1755,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="A1" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -1813,528 +1775,558 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="50" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="52"/>
+      <c r="B5" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C5" s="51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="17" t="s">
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="52"/>
+      <c r="B6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C6" s="51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
-      <c r="B6" s="17" t="s">
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="B7" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="52"/>
+      <c r="B8" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="49" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+      <c r="B9" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="52"/>
+      <c r="B10" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="C10" s="51" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="52"/>
+      <c r="B11" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C11" s="51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="17" t="s">
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="52"/>
+      <c r="B12" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C12" s="51" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="52"/>
+      <c r="B13" s="50" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+      <c r="C13" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="17" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="52"/>
+      <c r="B14" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C14" s="51" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
-      <c r="B10" s="17" t="s">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="52"/>
+      <c r="B15" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C15" s="51" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
-      <c r="B11" s="17" t="s">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="B16" s="50" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
-      <c r="B12" s="17" t="s">
+      <c r="C16" s="51" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" s="52"/>
+      <c r="B17" s="50" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="52"/>
+      <c r="B18" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
-      <c r="B13" s="17" t="s">
+      <c r="C18" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="18" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="49" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="42"/>
-      <c r="B14" s="17" t="s">
+      <c r="B19" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="49"/>
+      <c r="B20" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C20" s="51" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="42"/>
-      <c r="B15" s="17" t="s">
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A21" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="49" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+      <c r="B22" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="C22" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="18" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="52"/>
+      <c r="B23" s="50" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="42"/>
-      <c r="B17" s="17" t="s">
+      <c r="C23" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="18" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A24" s="53" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="42"/>
-      <c r="B18" s="17" t="s">
+      <c r="B24" s="54"/>
+      <c r="C24" s="55"/>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="B25" s="50" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="C25" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="17" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="52"/>
+      <c r="B26" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C26" s="51" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="52"/>
+      <c r="B27" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="18"/>
-    </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="41" t="s">
+      <c r="C27" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="17" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="52"/>
+      <c r="B28" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C28" s="51" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="52"/>
+      <c r="B29" s="50" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="42"/>
-      <c r="B22" s="17" t="s">
+      <c r="C29" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="18" t="s">
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="52"/>
+      <c r="B30" s="50" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="C30" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="18"/>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="41" t="s">
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="52"/>
+      <c r="B31" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="C31" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="18" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A32" s="53" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="42"/>
-      <c r="B25" s="17" t="s">
+      <c r="B32" s="54"/>
+      <c r="C32" s="55"/>
+    </row>
+    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A33" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="B33" s="54"/>
+      <c r="C33" s="55"/>
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="42"/>
-      <c r="B26" s="17" t="s">
+      <c r="B34" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C34" s="51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="42"/>
-      <c r="B27" s="17" t="s">
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="52"/>
+      <c r="B35" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C35" s="51" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="42"/>
-      <c r="B28" s="17" t="s">
+    <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="B36" s="50" t="s">
+        <v>247</v>
+      </c>
+      <c r="C36" s="51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="42"/>
-      <c r="B29" s="17" t="s">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="52"/>
+      <c r="B37" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C37" s="51" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="42"/>
-      <c r="B30" s="17" t="s">
+    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A38" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="B38" s="50" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="s">
+      <c r="C38" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="18"/>
-    </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
+    </row>
+    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A39" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="18"/>
-    </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="41" t="s">
+      <c r="B39" s="54"/>
+      <c r="C39" s="55"/>
+    </row>
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B40" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C40" s="51" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="52"/>
+      <c r="B41" s="50" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
-      <c r="B34" s="17" t="s">
+      <c r="C41" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="18" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A42" s="52"/>
+      <c r="B42" s="50" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="41" t="s">
+      <c r="C42" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="17" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" s="52"/>
+      <c r="B43" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C43" s="51" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="52"/>
+      <c r="B44" s="50" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="42"/>
-      <c r="B36" s="17" t="s">
+      <c r="C44" s="51"/>
+    </row>
+    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A45" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="B45" s="54"/>
+      <c r="C45" s="55"/>
+    </row>
+    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A46" s="53" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="B46" s="54"/>
+      <c r="C46" s="55"/>
+    </row>
+    <row r="47" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A47" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B47" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="C47" s="51" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="49"/>
+      <c r="B48" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C48" s="51" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
+    <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="49"/>
+      <c r="B49" s="50" t="s">
+        <v>251</v>
+      </c>
+      <c r="C49" s="51" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="49"/>
+      <c r="B50" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="18"/>
-    </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="41" t="s">
+      <c r="C50" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="17" t="s">
+    </row>
+    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" s="49"/>
+      <c r="B51" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="C51" s="51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="B52" s="50" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="42"/>
-      <c r="B40" s="17" t="s">
+      <c r="C52" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="18" t="s">
+    </row>
+    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="49"/>
+      <c r="B53" s="50" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A41" s="42"/>
-      <c r="B41" s="17" t="s">
+      <c r="C53" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C41" s="18" t="s">
+    </row>
+    <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="49"/>
+      <c r="B54" s="50" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="85" x14ac:dyDescent="0.2">
-      <c r="A42" s="42"/>
-      <c r="B42" s="17" t="s">
+      <c r="C54" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="42"/>
-      <c r="B43" s="17" t="s">
+    </row>
+    <row r="55" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="49"/>
+      <c r="B55" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="18"/>
-    </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
+      <c r="C55" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="18"/>
-    </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A45" s="19" t="s">
+    </row>
+    <row r="56" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" s="49"/>
+      <c r="B56" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="18"/>
-    </row>
-    <row r="46" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
+      <c r="C56" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="B46" s="17" t="s">
+    </row>
+    <row r="57" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A57" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="B57" s="50" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
-      <c r="B47" s="17" t="s">
+      <c r="C57" s="51" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A58" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="B58" s="54"/>
+      <c r="C58" s="55"/>
+    </row>
+    <row r="59" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A59" s="53" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="20"/>
-      <c r="B48" s="17" t="s">
+      <c r="B59" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
+      <c r="C59" s="51" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A60" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B60" s="50"/>
+      <c r="C60" s="56"/>
+    </row>
+    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A61" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="B61" s="50"/>
+      <c r="C61" s="51"/>
+    </row>
+    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A62" s="53" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A50" s="20"/>
-      <c r="B50" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="20"/>
-      <c r="B51" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="20"/>
-      <c r="B52" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="20"/>
-      <c r="B53" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="18"/>
-    </row>
-    <row r="56" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A56" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="18"/>
-    </row>
-    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A58" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="18"/>
-    </row>
-    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A59" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="18"/>
+      <c r="B62" s="54"/>
+      <c r="C62" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A25:A31"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A47:A51"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A39:A43"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2367,30 +2359,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2429,8 +2421,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>221</v>
+      <c r="A1" s="16" t="s">
+        <v>201</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2443,36 +2435,36 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2507,257 +2499,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="22">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="38">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="39"/>
+      <c r="B6" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="40"/>
+      <c r="B7" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="38">
+        <v>3</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="39"/>
+      <c r="B9" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="40"/>
+      <c r="B10" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="26" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="38">
+        <v>2</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D11" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="26" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="39"/>
+      <c r="B12" s="15" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="27">
+      <c r="C12" s="36"/>
+      <c r="D12" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="40"/>
+      <c r="B13" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="38">
+        <v>1</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="39"/>
+      <c r="B15" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="40"/>
+      <c r="B16" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="20" spans="1:4" ht="126" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A21" s="23">
         <v>5</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="46">
+      <c r="B21" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A22" s="23">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="47"/>
-      <c r="B6" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="48"/>
-      <c r="B7" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="46">
+      <c r="B22" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A23" s="23">
         <v>3</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="47"/>
-      <c r="B9" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="48"/>
-      <c r="B10" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="46">
+      <c r="B23" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A24" s="23">
         <v>2</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
-      <c r="B12" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="48"/>
-      <c r="B13" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="46">
+      <c r="B24" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A25" s="23">
         <v>1</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="47"/>
-      <c r="B15" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
-      <c r="B16" s="18" t="s">
+      <c r="B25" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="18" t="s">
+      <c r="C25" s="15" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="20" spans="1:4" ht="126" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="D25" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A21" s="28">
-        <v>5</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="28">
-        <v>4</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" s="28">
-        <v>3</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A24" s="28">
-        <v>2</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="28">
-        <v>1</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2798,15 +2790,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="A1" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -2817,37 +2809,37 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="52" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
+      <c r="C3" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>165</v>
+      <c r="C4" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
-        <v>166</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>168</v>
+      <c r="A5" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>151</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="6"/>
@@ -2856,9 +2848,9 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="29" t="s">
-        <v>169</v>
+      <c r="A6" s="42"/>
+      <c r="B6" s="24" t="s">
+        <v>152</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="3"/>
@@ -2867,9 +2859,9 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
-      <c r="B7" s="29" t="s">
-        <v>170</v>
+      <c r="A7" s="42"/>
+      <c r="B7" s="24" t="s">
+        <v>153</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="3"/>
@@ -2878,9 +2870,9 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
-      <c r="B8" s="29" t="s">
-        <v>171</v>
+      <c r="A8" s="42"/>
+      <c r="B8" s="24" t="s">
+        <v>154</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2889,9 +2881,9 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
-      <c r="B9" s="29" t="s">
-        <v>172</v>
+      <c r="A9" s="43"/>
+      <c r="B9" s="24" t="s">
+        <v>155</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2942,104 +2934,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>222</v>
+      <c r="A1" s="17" t="s">
+        <v>202</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J2" s="12" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J3" s="13" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J4" s="10" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J5" s="14" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>212</v>
-      </c>
       <c r="L7" s="9" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3074,33 +3066,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include risk level in Unresolved Anomalies sheet Include numerical risk levels from SOP-0006 rev 7 in Risk Matrix sheet
</commit_message>
<xml_diff>
--- a/templates/excel/fda-template.xlsx
+++ b/templates/excel/fda-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11C277B-D921-A64B-8E29-5951817E7667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7C6287-A39F-104B-8CBA-3B515AEC50A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" activeTab="7" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
+    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="16" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Unresolved Anomalies" sheetId="12" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Unresolved Anomalies'!$A$3:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Unresolved Anomalies'!$A$3:$F$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="257">
   <si>
     <t>Term</t>
   </si>
@@ -812,13 +812,16 @@
   </si>
   <si>
     <t>Feature telling Tidepool Loop to adjust both your basal insulin and your glucose CORRECTION_RANGE to help you meet your glucose goals during that activity. Workout temp adjust will be in effect for the time you indicate when you activate it or until you cancel it.</t>
+  </si>
+  <si>
+    <t>Risk Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -937,6 +940,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -1074,21 +1083,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1160,6 +1158,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1223,6 +1224,21 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1543,7 +1559,7 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1555,161 +1571,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="35"/>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
     </row>
     <row r="3" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
     </row>
     <row r="4" spans="1:3" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="31"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="C8" s="35"/>
-    </row>
-    <row r="9" spans="1:3" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+      <c r="C8" s="31"/>
+    </row>
+    <row r="9" spans="1:3" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-    </row>
-    <row r="10" spans="1:3" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+    </row>
+    <row r="10" spans="1:3" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:3" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="3" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="3" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="3" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="3" t="s">
         <v>225</v>
       </c>
     </row>
@@ -1755,562 +1771,562 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="25" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="44"/>
-      <c r="B5" s="29" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
-      <c r="B6" s="29" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="25" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="25" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="40"/>
+      <c r="B8" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="25" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="25" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
-      <c r="B10" s="29" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="25" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="29" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="25" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
-      <c r="B12" s="29" t="s">
+      <c r="A12" s="40"/>
+      <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="25" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="40"/>
+      <c r="B13" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="25" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="29" t="s">
+      <c r="A14" s="40"/>
+      <c r="B14" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
-      <c r="B15" s="29" t="s">
+      <c r="A15" s="40"/>
+      <c r="B15" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="25" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="25" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
-      <c r="B17" s="29" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="24" t="s">
         <v>242</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="25" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="40"/>
+      <c r="B18" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="25" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="25" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
-      <c r="B20" s="29" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="25" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="25" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="29" t="s">
+      <c r="A23" s="40"/>
+      <c r="B23" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="25" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="25" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="29" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="25" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="29" t="s">
+      <c r="A27" s="40"/>
+      <c r="B27" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="25" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="29" t="s">
+      <c r="A28" s="40"/>
+      <c r="B28" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="25" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
-      <c r="B29" s="29" t="s">
+      <c r="A29" s="40"/>
+      <c r="B29" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="25" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="29" t="s">
+      <c r="A30" s="40"/>
+      <c r="B30" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="29" t="s">
+      <c r="A31" s="40"/>
+      <c r="B31" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="33"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
     </row>
     <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="33"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="28"/>
     </row>
     <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="25" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="44"/>
-      <c r="B35" s="29" t="s">
+      <c r="A35" s="40"/>
+      <c r="B35" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="25" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="25" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="44"/>
-      <c r="B37" s="29" t="s">
+      <c r="A37" s="40"/>
+      <c r="B37" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="25" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="25" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="33"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="28"/>
     </row>
     <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="25" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="44"/>
-      <c r="B41" s="29" t="s">
+      <c r="A41" s="40"/>
+      <c r="B41" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="25" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A42" s="44"/>
-      <c r="B42" s="29" t="s">
+      <c r="A42" s="40"/>
+      <c r="B42" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="25" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A43" s="44"/>
-      <c r="B43" s="29" t="s">
+      <c r="A43" s="40"/>
+      <c r="B43" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="30" t="s">
+      <c r="C43" s="25" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="44"/>
-      <c r="B44" s="29" t="s">
+      <c r="A44" s="40"/>
+      <c r="B44" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="30"/>
+      <c r="C44" s="25"/>
     </row>
     <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="33"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
     </row>
     <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="32"/>
-      <c r="C46" s="33"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="28"/>
     </row>
     <row r="47" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A47" s="42" t="s">
+      <c r="A47" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="25" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="42"/>
-      <c r="B48" s="29" t="s">
+      <c r="A48" s="38"/>
+      <c r="B48" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="42"/>
-      <c r="B49" s="29" t="s">
+      <c r="A49" s="38"/>
+      <c r="B49" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="25" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="42"/>
-      <c r="B50" s="29" t="s">
+      <c r="A50" s="38"/>
+      <c r="B50" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C50" s="25" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="42"/>
-      <c r="B51" s="29" t="s">
+      <c r="A51" s="38"/>
+      <c r="B51" s="24" t="s">
         <v>253</v>
       </c>
-      <c r="C51" s="30" t="s">
+      <c r="C51" s="25" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A52" s="42" t="s">
+      <c r="A52" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C52" s="30" t="s">
+      <c r="C52" s="25" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="42"/>
-      <c r="B53" s="29" t="s">
+      <c r="A53" s="38"/>
+      <c r="B53" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="25" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="42"/>
-      <c r="B54" s="29" t="s">
+      <c r="A54" s="38"/>
+      <c r="B54" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="25" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="42"/>
-      <c r="B55" s="29" t="s">
+      <c r="A55" s="38"/>
+      <c r="B55" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C55" s="30" t="s">
+      <c r="C55" s="25" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="42"/>
-      <c r="B56" s="29" t="s">
+      <c r="A56" s="38"/>
+      <c r="B56" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="25" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C57" s="30" t="s">
+      <c r="C57" s="25" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A58" s="31" t="s">
+      <c r="A58" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="33"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="28"/>
     </row>
     <row r="59" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A59" s="31" t="s">
+      <c r="A59" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="B59" s="29" t="s">
+      <c r="B59" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="C59" s="30" t="s">
+      <c r="C59" s="25" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A60" s="31" t="s">
+      <c r="A60" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="34"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="29"/>
     </row>
     <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="30"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="25"/>
     </row>
     <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A62" s="31" t="s">
+      <c r="A62" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B62" s="32"/>
-      <c r="C62" s="33"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2357,24 +2373,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2417,7 +2433,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>201</v>
       </c>
       <c r="B1" s="2"/>
@@ -2430,31 +2446,31 @@
       <c r="I1" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="4" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2493,256 +2509,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="22">
+      <c r="A4" s="17">
         <v>5</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="48">
+      <c r="A5" s="44">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="49"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="10" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="46"/>
+      <c r="B7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="15" t="s">
+      <c r="C7" s="43"/>
+      <c r="D7" s="10" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="48">
+      <c r="A8" s="44">
         <v>3</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="10" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="42"/>
+      <c r="D9" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="50"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="10" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="48">
+      <c r="A11" s="44">
         <v>2</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="45" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="10" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="15" t="s">
+      <c r="C12" s="42"/>
+      <c r="D12" s="10" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="50"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="46"/>
+      <c r="B13" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="43"/>
+      <c r="D13" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="48">
+      <c r="A14" s="44">
         <v>1</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="45" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="10" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="15" t="s">
+      <c r="C15" s="42"/>
+      <c r="D15" s="10" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="50"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="46"/>
+      <c r="B16" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="15" t="s">
+      <c r="C16" s="43"/>
+      <c r="D16" s="10" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
     </row>
     <row r="20" spans="1:4" ht="126" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="16" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A21" s="23">
+      <c r="A21" s="18">
         <v>5</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="10" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="23">
+      <c r="A22" s="18">
         <v>4</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="10" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" s="23">
+      <c r="A23" s="18">
         <v>3</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A24" s="23">
+      <c r="A24" s="18">
         <v>2</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="23">
+      <c r="A25" s="18">
         <v>1</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="10" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2782,15 +2798,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -2801,87 +2817,137 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="52"/>
     </row>
     <row r="4" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="20" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
+      <c r="C5" s="53">
+        <v>5</v>
+      </c>
+      <c r="D5" s="54">
+        <v>10</v>
+      </c>
+      <c r="E5" s="54">
+        <v>13</v>
+      </c>
+      <c r="F5" s="54">
+        <v>20</v>
+      </c>
+      <c r="G5" s="55">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="48"/>
+      <c r="B6" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
+      <c r="C6" s="56">
+        <v>4</v>
+      </c>
+      <c r="D6" s="53">
+        <v>8</v>
+      </c>
+      <c r="E6" s="54">
+        <v>12</v>
+      </c>
+      <c r="F6" s="54">
+        <v>16</v>
+      </c>
+      <c r="G6" s="55">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="48"/>
+      <c r="B7" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
+      <c r="C7" s="56">
+        <v>3</v>
+      </c>
+      <c r="D7" s="53">
+        <v>6</v>
+      </c>
+      <c r="E7" s="53">
+        <v>9</v>
+      </c>
+      <c r="F7" s="54">
+        <v>12</v>
+      </c>
+      <c r="G7" s="55">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="48"/>
+      <c r="B8" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="7"/>
+      <c r="C8" s="56">
+        <v>2</v>
+      </c>
+      <c r="D8" s="56">
+        <v>4</v>
+      </c>
+      <c r="E8" s="53">
+        <v>6</v>
+      </c>
+      <c r="F8" s="53">
+        <v>8</v>
+      </c>
+      <c r="G8" s="55">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="49"/>
+      <c r="B9" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
+      <c r="C9" s="56">
+        <v>1</v>
+      </c>
+      <c r="D9" s="56">
+        <v>2</v>
+      </c>
+      <c r="E9" s="56">
+        <v>3</v>
+      </c>
+      <c r="F9" s="53">
+        <v>4</v>
+      </c>
+      <c r="G9" s="57">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2924,98 +2990,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="6" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="7" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="8" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="5" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="P5" s="9" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="4" t="s">
         <v>199</v>
       </c>
     </row>
@@ -3040,9 +3106,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3053,38 +3121,41 @@
     <col min="5" max="5" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>227</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E3" xr:uid="{AF851B01-A62E-CF4F-B7DC-5677CB269975}"/>
+  <autoFilter ref="A3:F4" xr:uid="{CD4B26C9-B562-5744-A608-BA787B1192D0}"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Remove "Benefit" column from Hazard Analysis sheet
</commit_message>
<xml_diff>
--- a/templates/excel/fda-template.xlsx
+++ b/templates/excel/fda-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7C6287-A39F-104B-8CBA-3B515AEC50A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B196C4C-A1F6-0946-9313-5CBD162CD152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="256">
   <si>
     <t>Term</t>
   </si>
@@ -641,9 +641,6 @@
   </si>
   <si>
     <t>Residual Risk Score</t>
-  </si>
-  <si>
-    <t>Benefit outweigh Risks? Y/N</t>
   </si>
   <si>
     <t>Software Requirements</t>
@@ -1161,6 +1158,21 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1183,12 +1195,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1224,21 +1236,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1571,162 +1568,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
     </row>
     <row r="4" spans="1:3" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
-        <v>217</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="C5" s="31"/>
+        <v>206</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="C6" s="31"/>
+        <v>206</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="36"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="C7" s="31"/>
+        <v>206</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="36"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="C8" s="31"/>
+        <v>206</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" s="36"/>
     </row>
     <row r="9" spans="1:3" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
+      <c r="A9" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
     </row>
     <row r="10" spans="1:3" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="42" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="42" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -1771,11 +1768,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
@@ -1792,18 +1789,18 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="43" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="24" t="s">
         <v>3</v>
       </c>
@@ -1812,7 +1809,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="24" t="s">
         <v>5</v>
       </c>
@@ -1821,47 +1818,47 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="C7" s="25" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="44"/>
+      <c r="B8" s="24" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
-      <c r="B8" s="24" t="s">
+      <c r="C8" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="C8" s="25" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>237</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>238</v>
-      </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="24" t="s">
         <v>10</v>
       </c>
@@ -1870,16 +1867,16 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
+      <c r="A13" s="44"/>
       <c r="B13" s="24" t="s">
         <v>13</v>
       </c>
@@ -1888,7 +1885,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="24" t="s">
         <v>15</v>
       </c>
@@ -1897,7 +1894,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="24" t="s">
         <v>17</v>
       </c>
@@ -1906,27 +1903,27 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="43" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="24" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-      <c r="B17" s="24" t="s">
+      <c r="C17" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>243</v>
-      </c>
     </row>
     <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="40"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="24" t="s">
         <v>21</v>
       </c>
@@ -1935,18 +1932,18 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="43" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>245</v>
-      </c>
     </row>
     <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="24" t="s">
         <v>24</v>
       </c>
@@ -1962,7 +1959,7 @@
       <c r="C21" s="28"/>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="24" t="s">
@@ -1973,7 +1970,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="40"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="24" t="s">
         <v>30</v>
       </c>
@@ -1989,7 +1986,7 @@
       <c r="C24" s="28"/>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="43" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="24" t="s">
@@ -2000,7 +1997,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="40"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="24" t="s">
         <v>36</v>
       </c>
@@ -2009,7 +2006,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="40"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="24" t="s">
         <v>38</v>
       </c>
@@ -2018,16 +2015,16 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="40"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="40"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="24" t="s">
         <v>41</v>
       </c>
@@ -2036,7 +2033,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
+      <c r="A30" s="44"/>
       <c r="B30" s="24" t="s">
         <v>43</v>
       </c>
@@ -2045,7 +2042,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="40"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="24" t="s">
         <v>45</v>
       </c>
@@ -2068,7 +2065,7 @@
       <c r="C33" s="28"/>
     </row>
     <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="43" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -2079,7 +2076,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="40"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="24" t="s">
         <v>52</v>
       </c>
@@ -2088,18 +2085,18 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="43" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C36" s="25" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="40"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="24" t="s">
         <v>56</v>
       </c>
@@ -2126,18 +2123,18 @@
       <c r="C39" s="28"/>
     </row>
     <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="43" t="s">
         <v>62</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>63</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="40"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="24" t="s">
         <v>64</v>
       </c>
@@ -2146,7 +2143,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A42" s="40"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="24" t="s">
         <v>66</v>
       </c>
@@ -2155,16 +2152,16 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A43" s="40"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="24" t="s">
         <v>68</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="40"/>
+      <c r="A44" s="44"/>
       <c r="B44" s="24" t="s">
         <v>69</v>
       </c>
@@ -2185,18 +2182,18 @@
       <c r="C46" s="28"/>
     </row>
     <row r="47" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="43" t="s">
         <v>72</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="38"/>
+      <c r="A48" s="43"/>
       <c r="B48" s="24" t="s">
         <v>73</v>
       </c>
@@ -2205,16 +2202,16 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="38"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="C49" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="C49" s="25" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="38"/>
+      <c r="A50" s="43"/>
       <c r="B50" s="24" t="s">
         <v>75</v>
       </c>
@@ -2223,16 +2220,16 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="38"/>
+      <c r="A51" s="43"/>
       <c r="B51" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C51" s="25" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="43" t="s">
         <v>77</v>
       </c>
       <c r="B52" s="24" t="s">
@@ -2243,7 +2240,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="38"/>
+      <c r="A53" s="43"/>
       <c r="B53" s="24" t="s">
         <v>80</v>
       </c>
@@ -2252,7 +2249,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="38"/>
+      <c r="A54" s="43"/>
       <c r="B54" s="24" t="s">
         <v>82</v>
       </c>
@@ -2261,7 +2258,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="38"/>
+      <c r="A55" s="43"/>
       <c r="B55" s="24" t="s">
         <v>84</v>
       </c>
@@ -2270,7 +2267,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="38"/>
+      <c r="A56" s="43"/>
       <c r="B56" s="24" t="s">
         <v>86</v>
       </c>
@@ -2286,7 +2283,7 @@
         <v>89</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.2">
@@ -2304,7 +2301,7 @@
         <v>92</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.2">
@@ -2330,6 +2327,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A16:A18"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A25:A31"/>
@@ -2337,12 +2340,6 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2374,7 +2371,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -2396,7 +2393,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2434,7 +2431,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2476,7 +2473,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2543,11 +2540,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="44">
+      <c r="A5" s="49">
         <v>4</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="46" t="s">
         <v>102</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -2555,31 +2552,31 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="45"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="10" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="10" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="44">
+      <c r="A8" s="49">
         <v>3</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="46" t="s">
         <v>108</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -2587,31 +2584,31 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="45"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="43"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="10" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="44">
+      <c r="A11" s="49">
         <v>2</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="46" t="s">
         <v>114</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -2619,31 +2616,31 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="45"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="42"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="10" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="43"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="44">
+      <c r="A14" s="49">
         <v>1</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="46" t="s">
         <v>120</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -2651,21 +2648,21 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="45"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="42"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="10" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="43"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="10" t="s">
         <v>125</v>
       </c>
@@ -2817,13 +2814,13 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="52"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="20" t="s">
@@ -2843,109 +2840,109 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="52" t="s">
         <v>149</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="31">
         <v>5</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="32">
         <v>10</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="32">
         <v>13</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="32">
         <v>20</v>
       </c>
-      <c r="G5" s="55">
+      <c r="G5" s="33">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="48"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="34">
         <v>4</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="31">
         <v>8</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="32">
         <v>12</v>
       </c>
-      <c r="F6" s="54">
+      <c r="F6" s="32">
         <v>16</v>
       </c>
-      <c r="G6" s="55">
+      <c r="G6" s="33">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="48"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="34">
         <v>3</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="31">
         <v>6</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="31">
         <v>9</v>
       </c>
-      <c r="F7" s="54">
+      <c r="F7" s="32">
         <v>12</v>
       </c>
-      <c r="G7" s="55">
+      <c r="G7" s="33">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C8" s="56">
+      <c r="C8" s="34">
         <v>2</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="34">
         <v>4</v>
       </c>
-      <c r="E8" s="53">
+      <c r="E8" s="31">
         <v>6</v>
       </c>
-      <c r="F8" s="53">
+      <c r="F8" s="31">
         <v>8</v>
       </c>
-      <c r="G8" s="55">
+      <c r="G8" s="33">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="56">
+      <c r="C9" s="34">
         <v>1</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="34">
         <v>2</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="34">
         <v>3</v>
       </c>
-      <c r="F9" s="53">
+      <c r="F9" s="31">
         <v>4</v>
       </c>
-      <c r="G9" s="57">
+      <c r="G9" s="35">
         <v>5</v>
       </c>
     </row>
@@ -2969,7 +2966,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2986,12 +2983,11 @@
     <col min="12" max="13" width="50.6640625" customWidth="1"/>
     <col min="14" max="15" width="12.6640625" customWidth="1"/>
     <col min="16" max="16" width="11.6640625" customWidth="1"/>
-    <col min="17" max="17" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="28" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>176</v>
@@ -3000,7 +2996,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J2" s="7" t="s">
         <v>178</v>
       </c>
@@ -3008,7 +3004,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J3" s="8" t="s">
         <v>180</v>
       </c>
@@ -3016,7 +3012,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J4" s="5" t="s">
         <v>182</v>
       </c>
@@ -3024,7 +3020,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J5" s="9" t="s">
         <v>184</v>
       </c>
@@ -3032,7 +3028,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>173</v>
       </c>
@@ -3081,13 +3077,10 @@
       <c r="P7" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="Q7" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3123,7 +3116,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="25" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -3131,10 +3124,10 @@
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>229</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>168</v>
@@ -3143,15 +3136,15 @@
         <v>169</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-created Verification Test Report (formerly "Epics", though this has does not list epics) for Appendix 16.2
</commit_message>
<xml_diff>
--- a/templates/excel/fda-template.xlsx
+++ b/templates/excel/fda-template.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tapani/src/tidepool/reports/templates/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B196C4C-A1F6-0946-9313-5CBD162CD152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CABF32E-AFF5-A64C-89DD-5AAA96D9998F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
+    <workbookView xWindow="860" yWindow="1100" windowWidth="31380" windowHeight="16940" activeTab="4" xr2:uid="{65B606C8-7B73-2B4A-9146-6FF011B77E80}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="16" r:id="rId1"/>
     <sheet name="Glossary" sheetId="17" r:id="rId2"/>
     <sheet name="Software Requirements" sheetId="6" r:id="rId3"/>
     <sheet name="Traceability Report" sheetId="14" r:id="rId4"/>
-    <sheet name="Risk Scoring" sheetId="2" r:id="rId5"/>
-    <sheet name="Risk Matrix" sheetId="3" r:id="rId6"/>
-    <sheet name="Hazard Analysis" sheetId="10" r:id="rId7"/>
-    <sheet name="Unresolved Anomalies" sheetId="12" r:id="rId8"/>
+    <sheet name="Verification Test Report" sheetId="18" r:id="rId5"/>
+    <sheet name="Risk Scoring" sheetId="2" r:id="rId6"/>
+    <sheet name="Risk Matrix" sheetId="3" r:id="rId7"/>
+    <sheet name="Hazard Analysis" sheetId="10" r:id="rId8"/>
+    <sheet name="Unresolved Anomalies" sheetId="12" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Unresolved Anomalies'!$A$3:$F$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Unresolved Anomalies'!$A$3:$F$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="258">
   <si>
     <t>Term</t>
   </si>
@@ -812,6 +813,12 @@
   </si>
   <si>
     <t>Risk Level</t>
+  </si>
+  <si>
+    <t>Verification Test Report</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;insert: verification_report()&gt;&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1087,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1173,6 +1180,7 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1195,11 +1203,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1556,7 +1564,7 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1568,75 +1576,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
     </row>
     <row r="3" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
     </row>
     <row r="4" spans="1:3" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="37"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="37"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="37"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="37"/>
     </row>
     <row r="9" spans="1:3" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
     </row>
     <row r="10" spans="1:3" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
@@ -1789,7 +1797,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="44" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="24" t="s">
@@ -1800,7 +1808,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="44"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="24" t="s">
         <v>3</v>
       </c>
@@ -1809,7 +1817,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="44"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="24" t="s">
         <v>5</v>
       </c>
@@ -1818,7 +1826,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="24" t="s">
@@ -1829,7 +1837,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="44"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="24" t="s">
         <v>234</v>
       </c>
@@ -1838,7 +1846,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
@@ -1849,7 +1857,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="44"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="24" t="s">
         <v>9</v>
       </c>
@@ -1858,7 +1866,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="44"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="24" t="s">
         <v>10</v>
       </c>
@@ -1867,7 +1875,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="44"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
@@ -1876,7 +1884,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="24" t="s">
         <v>13</v>
       </c>
@@ -1885,7 +1893,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="44"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="24" t="s">
         <v>15</v>
       </c>
@@ -1894,7 +1902,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="44"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="24" t="s">
         <v>17</v>
       </c>
@@ -1903,7 +1911,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="44" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="24" t="s">
@@ -1914,7 +1922,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="44"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="24" t="s">
         <v>241</v>
       </c>
@@ -1923,7 +1931,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="44"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="24" t="s">
         <v>21</v>
       </c>
@@ -1932,7 +1940,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="24" t="s">
@@ -1943,7 +1951,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A20" s="43"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="24" t="s">
         <v>24</v>
       </c>
@@ -1959,7 +1967,7 @@
       <c r="C21" s="28"/>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="44" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="24" t="s">
@@ -1970,7 +1978,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="44"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="24" t="s">
         <v>30</v>
       </c>
@@ -1986,7 +1994,7 @@
       <c r="C24" s="28"/>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="44" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="24" t="s">
@@ -1997,7 +2005,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="44"/>
+      <c r="A26" s="46"/>
       <c r="B26" s="24" t="s">
         <v>36</v>
       </c>
@@ -2006,7 +2014,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="44"/>
+      <c r="A27" s="46"/>
       <c r="B27" s="24" t="s">
         <v>38</v>
       </c>
@@ -2015,7 +2023,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="44"/>
+      <c r="A28" s="46"/>
       <c r="B28" s="24" t="s">
         <v>40</v>
       </c>
@@ -2024,7 +2032,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="44"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="24" t="s">
         <v>41</v>
       </c>
@@ -2033,7 +2041,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="44"/>
+      <c r="A30" s="46"/>
       <c r="B30" s="24" t="s">
         <v>43</v>
       </c>
@@ -2042,7 +2050,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="44"/>
+      <c r="A31" s="46"/>
       <c r="B31" s="24" t="s">
         <v>45</v>
       </c>
@@ -2065,7 +2073,7 @@
       <c r="C33" s="28"/>
     </row>
     <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="44" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="24" t="s">
@@ -2076,7 +2084,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="44"/>
+      <c r="A35" s="46"/>
       <c r="B35" s="24" t="s">
         <v>52</v>
       </c>
@@ -2085,7 +2093,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="44" t="s">
         <v>54</v>
       </c>
       <c r="B36" s="24" t="s">
@@ -2096,7 +2104,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="44"/>
+      <c r="A37" s="46"/>
       <c r="B37" s="24" t="s">
         <v>56</v>
       </c>
@@ -2123,7 +2131,7 @@
       <c r="C39" s="28"/>
     </row>
     <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="43" t="s">
+      <c r="A40" s="44" t="s">
         <v>62</v>
       </c>
       <c r="B40" s="24" t="s">
@@ -2134,7 +2142,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="44"/>
+      <c r="A41" s="46"/>
       <c r="B41" s="24" t="s">
         <v>64</v>
       </c>
@@ -2143,7 +2151,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A42" s="44"/>
+      <c r="A42" s="46"/>
       <c r="B42" s="24" t="s">
         <v>66</v>
       </c>
@@ -2152,7 +2160,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A43" s="44"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="24" t="s">
         <v>68</v>
       </c>
@@ -2161,7 +2169,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="44"/>
+      <c r="A44" s="46"/>
       <c r="B44" s="24" t="s">
         <v>69</v>
       </c>
@@ -2182,7 +2190,7 @@
       <c r="C46" s="28"/>
     </row>
     <row r="47" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="44" t="s">
         <v>72</v>
       </c>
       <c r="B47" s="24" t="s">
@@ -2193,7 +2201,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A48" s="43"/>
+      <c r="A48" s="44"/>
       <c r="B48" s="24" t="s">
         <v>73</v>
       </c>
@@ -2202,7 +2210,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="43"/>
+      <c r="A49" s="44"/>
       <c r="B49" s="24" t="s">
         <v>250</v>
       </c>
@@ -2211,7 +2219,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="43"/>
+      <c r="A50" s="44"/>
       <c r="B50" s="24" t="s">
         <v>75</v>
       </c>
@@ -2220,7 +2228,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A51" s="43"/>
+      <c r="A51" s="44"/>
       <c r="B51" s="24" t="s">
         <v>252</v>
       </c>
@@ -2229,7 +2237,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="44" t="s">
         <v>77</v>
       </c>
       <c r="B52" s="24" t="s">
@@ -2240,7 +2248,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="43"/>
+      <c r="A53" s="44"/>
       <c r="B53" s="24" t="s">
         <v>80</v>
       </c>
@@ -2249,7 +2257,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="43"/>
+      <c r="A54" s="44"/>
       <c r="B54" s="24" t="s">
         <v>82</v>
       </c>
@@ -2258,7 +2266,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="43"/>
+      <c r="A55" s="44"/>
       <c r="B55" s="24" t="s">
         <v>84</v>
       </c>
@@ -2267,7 +2275,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" s="43"/>
+      <c r="A56" s="44"/>
       <c r="B56" s="24" t="s">
         <v>86</v>
       </c>
@@ -2327,12 +2335,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A16:A18"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A25:A31"/>
@@ -2340,6 +2342,12 @@
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2488,6 +2496,69 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6CF2A0-08BE-4548-868F-43D1DF1EBA22}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="76.5" style="36" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="36" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="36" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>257</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="46" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter scaleWithDoc="0">
+    <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;K000000Tidepool Loop 1.0.0&amp;R&amp;"Calibri,Regular"&amp;K000000&amp;A</oddHeader>
+    <oddFooter>&amp;L&amp;"Calibri,Regular"&amp;K000000Generated on {timestamp}&amp;R&amp;"Calibri,Regular"&amp;K000000Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3948700B-C92F-8147-BAA1-9D18FBCBB7CE}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2540,11 +2611,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="49">
+      <c r="A5" s="50">
         <v>4</v>
       </c>
       <c r="B5" s="10"/>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="47" t="s">
         <v>102</v>
       </c>
       <c r="D5" s="10" t="s">
@@ -2552,31 +2623,31 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="10" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="51"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="10" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="49">
+      <c r="A8" s="50">
         <v>3</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="47" t="s">
         <v>108</v>
       </c>
       <c r="D8" s="10" t="s">
@@ -2584,31 +2655,31 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="47"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="48"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="10" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="49">
+      <c r="A11" s="50">
         <v>2</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="47" t="s">
         <v>114</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -2616,31 +2687,31 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="50"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="47"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="10" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="48"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="49">
+      <c r="A14" s="50">
         <v>1</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="47" t="s">
         <v>120</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -2648,21 +2719,21 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="50"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="47"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="10" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="48"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="10" t="s">
         <v>125</v>
       </c>
@@ -2780,7 +2851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6364E20A-6908-2147-AEE9-42144C5629EC}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2814,13 +2885,13 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="58"/>
     </row>
     <row r="4" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="20" t="s">
@@ -2840,7 +2911,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="53" t="s">
         <v>149</v>
       </c>
       <c r="B5" s="19" t="s">
@@ -2863,7 +2934,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="19" t="s">
         <v>152</v>
       </c>
@@ -2884,7 +2955,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="19" t="s">
         <v>153</v>
       </c>
@@ -2905,7 +2976,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="19" t="s">
         <v>154</v>
       </c>
@@ -2926,7 +2997,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="54"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="19" t="s">
         <v>155</v>
       </c>
@@ -2961,7 +3032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DB245F-55D2-7749-AB29-396B342A89D5}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3094,7 +3165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6FD87B-7E2F-6C44-96A8-401C1942CFED}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>